<commit_message>
Updated progress of sprint, sprint8
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint8.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint8.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16925"/>
-  <workbookPr defaultThemeVersion="164011"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\GIT\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\djnenadovic\Desktop\MATF\MasterAudioTechnologyFunctions\Documentation and designs\Sprint_info\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20496" windowHeight="7536" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Roster" sheetId="2" r:id="rId1"/>
     <sheet name="Sprint" sheetId="1" r:id="rId2"/>
     <sheet name="Chart" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="152511"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="49" uniqueCount="46">
   <si>
     <t>Name</t>
   </si>
@@ -156,12 +156,21 @@
   </si>
   <si>
     <t>Retest</t>
+  </si>
+  <si>
+    <t>To do</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>In progress</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.0"/>
   </numFmts>
@@ -345,24 +354,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -388,12 +379,6 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="3" applyBorder="1" applyAlignment="1">
@@ -405,6 +390,30 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="10" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="4">
     <cellStyle name="40% - Accent3" xfId="1" builtinId="39"/>
@@ -412,7 +421,22 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="4">
+  <dxfs count="7">
+    <dxf>
+      <font>
+        <color rgb="FFC00000"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="9" tint="-0.499984740745262"/>
+      </font>
+    </dxf>
+    <dxf>
+      <font>
+        <color theme="7" tint="-0.24994659260841701"/>
+      </font>
+    </dxf>
     <dxf>
       <font>
         <color theme="0"/>
@@ -452,7 +476,7 @@
 </file>
 
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -497,6 +521,7 @@
           </a:p>
         </c:rich>
       </c:tx>
+      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -528,7 +553,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -675,7 +700,7 @@
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000000-2B6F-4357-9072-E062BD4EF823}"/>
             </c:ext>
@@ -785,40 +810,40 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>6</c:v>
+                  <c:v>3</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:val>
           <c:smooth val="0"/>
-          <c:extLst>
+          <c:extLst xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-2B6F-4357-9072-E062BD4EF823}"/>
             </c:ext>
@@ -833,11 +858,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="308619040"/>
-        <c:axId val="308624616"/>
+        <c:axId val="278370696"/>
+        <c:axId val="278371872"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="308619040"/>
+        <c:axId val="278370696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -900,7 +925,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -937,10 +962,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308624616"/>
+        <c:crossAx val="278371872"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -948,7 +973,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="308624616"/>
+        <c:axId val="278371872"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -993,6 +1018,7 @@
               </a:p>
             </c:rich>
           </c:tx>
+          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1017,7 +1043,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="sr-Latn-RS"/>
+              <a:endParaRPr lang="en-US"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -1048,10 +1074,10 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="sr-Latn-RS"/>
+            <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="308619040"/>
+        <c:crossAx val="278370696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1099,7 +1125,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="sr-Latn-RS"/>
+          <a:endParaRPr lang="en-US"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1147,7 +1173,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="sr-Latn-RS"/>
+      <a:endParaRPr lang="en-US"/>
     </a:p>
   </c:txPr>
   <c:printSettings>
@@ -1714,7 +1740,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2040,64 +2066,64 @@
       <selection activeCell="D5" sqref="D5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18.85546875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.28515625" customWidth="1"/>
+    <col min="1" max="1" width="18.88671875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" s="10" t="s">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="12"/>
+      <c r="B1" s="23"/>
+      <c r="C1" s="23"/>
+      <c r="D1" s="24"/>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="C2" s="7"/>
+      <c r="C2" s="19"/>
       <c r="D2" s="3" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="20" t="s">
         <v>4</v>
       </c>
-      <c r="C3" s="8"/>
+      <c r="C3" s="20"/>
       <c r="D3" s="5" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" s="8" t="s">
+      <c r="B4" s="20" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="8"/>
+      <c r="C4" s="20"/>
       <c r="D4" s="5" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="C5" s="9"/>
+      <c r="C5" s="21"/>
       <c r="D5" s="6" t="s">
         <v>11</v>
       </c>
@@ -2119,453 +2145,461 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="24.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.5703125" style="13" customWidth="1"/>
-    <col min="3" max="3" width="13.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.28515625" style="13" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14" style="13" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.85546875" style="13" bestFit="1" customWidth="1"/>
-    <col min="7" max="15" width="5.7109375" style="13" customWidth="1"/>
-    <col min="16" max="19" width="6.7109375" style="13" customWidth="1"/>
-    <col min="20" max="20" width="6.7109375" style="13" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="10.42578125" style="13" bestFit="1" customWidth="1"/>
-    <col min="22" max="16384" width="9.140625" style="13"/>
+    <col min="1" max="1" width="24.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.5546875" style="7" customWidth="1"/>
+    <col min="3" max="3" width="13.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" style="7" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14" style="7" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.88671875" style="7" bestFit="1" customWidth="1"/>
+    <col min="7" max="15" width="5.6640625" style="7" customWidth="1"/>
+    <col min="16" max="19" width="6.6640625" style="7" customWidth="1"/>
+    <col min="20" max="20" width="6.6640625" style="7" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="10.44140625" style="7" bestFit="1" customWidth="1"/>
+    <col min="22" max="16384" width="9.109375" style="7"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B1" s="14" t="s">
+    <row r="1" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B1" s="8" t="s">
         <v>12</v>
       </c>
-      <c r="C1" s="15">
+      <c r="C1" s="9">
         <v>42548</v>
       </c>
-      <c r="E1" s="16"/>
-      <c r="F1" s="16"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
     </row>
-    <row r="2" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="B2" s="17" t="s">
+    <row r="2" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="B2" s="11" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="18">
+      <c r="C2" s="12">
         <f>C1+14</f>
         <v>42562</v>
       </c>
     </row>
-    <row r="4" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A4" s="19" t="s">
+    <row r="4" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A4" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="B4" s="19" t="s">
+      <c r="B4" s="13" t="s">
         <v>15</v>
       </c>
-      <c r="C4" s="19" t="s">
+      <c r="C4" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="19" t="s">
+      <c r="E4" s="13" t="s">
         <v>18</v>
       </c>
-      <c r="F4" s="20" t="s">
+      <c r="F4" s="14" t="s">
         <v>19</v>
       </c>
-      <c r="G4" s="19" t="s">
+      <c r="G4" s="13" t="s">
         <v>20</v>
       </c>
-      <c r="H4" s="19" t="s">
+      <c r="H4" s="13" t="s">
         <v>21</v>
       </c>
-      <c r="I4" s="19" t="s">
+      <c r="I4" s="13" t="s">
         <v>22</v>
       </c>
-      <c r="J4" s="19" t="s">
+      <c r="J4" s="13" t="s">
         <v>23</v>
       </c>
-      <c r="K4" s="19" t="s">
+      <c r="K4" s="13" t="s">
         <v>24</v>
       </c>
-      <c r="L4" s="19" t="s">
+      <c r="L4" s="13" t="s">
         <v>25</v>
       </c>
-      <c r="M4" s="19" t="s">
+      <c r="M4" s="13" t="s">
         <v>26</v>
       </c>
-      <c r="N4" s="19" t="s">
+      <c r="N4" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="O4" s="19" t="s">
+      <c r="O4" s="13" t="s">
         <v>28</v>
       </c>
-      <c r="P4" s="19" t="s">
+      <c r="P4" s="13" t="s">
         <v>29</v>
       </c>
-      <c r="Q4" s="19" t="s">
+      <c r="Q4" s="13" t="s">
         <v>30</v>
       </c>
-      <c r="R4" s="19" t="s">
+      <c r="R4" s="13" t="s">
         <v>31</v>
       </c>
-      <c r="S4" s="19" t="s">
+      <c r="S4" s="13" t="s">
         <v>32</v>
       </c>
-      <c r="T4" s="19" t="s">
+      <c r="T4" s="13" t="s">
         <v>33</v>
       </c>
-      <c r="U4" s="20" t="s">
+      <c r="U4" s="14" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+    <row r="5" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A5" s="26" t="s">
         <v>39</v>
       </c>
-      <c r="B5" s="22">
+      <c r="B5" s="25">
         <v>5</v>
       </c>
-      <c r="C5" s="23" t="s">
+      <c r="C5" s="15" t="s">
         <v>40</v>
       </c>
-      <c r="D5" s="23" t="s">
+      <c r="D5" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E5" s="23">
+      <c r="E5" s="15">
         <v>3</v>
       </c>
-      <c r="F5" s="23"/>
-      <c r="G5" s="23"/>
-      <c r="H5" s="23"/>
-      <c r="I5" s="23"/>
-      <c r="J5" s="23"/>
-      <c r="K5" s="23"/>
-      <c r="L5" s="23"/>
-      <c r="M5" s="23"/>
-      <c r="N5" s="23"/>
-      <c r="O5" s="23"/>
-      <c r="P5" s="23"/>
-      <c r="Q5" s="23"/>
-      <c r="R5" s="23"/>
-      <c r="S5" s="23"/>
-      <c r="T5" s="23"/>
-      <c r="U5" s="23">
+      <c r="F5" s="15" t="s">
+        <v>44</v>
+      </c>
+      <c r="G5" s="15"/>
+      <c r="H5" s="15"/>
+      <c r="I5" s="15"/>
+      <c r="J5" s="15"/>
+      <c r="K5" s="15">
+        <v>3</v>
+      </c>
+      <c r="L5" s="15"/>
+      <c r="M5" s="15"/>
+      <c r="N5" s="15"/>
+      <c r="O5" s="15"/>
+      <c r="P5" s="15"/>
+      <c r="Q5" s="15"/>
+      <c r="R5" s="15"/>
+      <c r="S5" s="15"/>
+      <c r="T5" s="15"/>
+      <c r="U5" s="15">
         <f>E5-SUM(G5:T5)</f>
-        <v>3</v>
+        <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A6" s="22"/>
-      <c r="B6" s="22"/>
-      <c r="C6" s="23" t="s">
+    <row r="6" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A6" s="25"/>
+      <c r="B6" s="25"/>
+      <c r="C6" s="15" t="s">
         <v>41</v>
       </c>
-      <c r="D6" s="23" t="s">
+      <c r="D6" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E6" s="23">
+      <c r="E6" s="15">
         <v>2</v>
       </c>
-      <c r="F6" s="23"/>
-      <c r="G6" s="23"/>
-      <c r="H6" s="23"/>
-      <c r="I6" s="23"/>
-      <c r="J6" s="23"/>
-      <c r="K6" s="23"/>
-      <c r="L6" s="23"/>
-      <c r="M6" s="23"/>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23"/>
-      <c r="P6" s="23"/>
-      <c r="Q6" s="23"/>
-      <c r="R6" s="23"/>
-      <c r="S6" s="23"/>
-      <c r="T6" s="23"/>
-      <c r="U6" s="23">
+      <c r="F6" s="15" t="s">
+        <v>45</v>
+      </c>
+      <c r="G6" s="15"/>
+      <c r="H6" s="15"/>
+      <c r="I6" s="15"/>
+      <c r="J6" s="15"/>
+      <c r="K6" s="15"/>
+      <c r="L6" s="15"/>
+      <c r="M6" s="15"/>
+      <c r="N6" s="15"/>
+      <c r="O6" s="15"/>
+      <c r="P6" s="15"/>
+      <c r="Q6" s="15"/>
+      <c r="R6" s="15"/>
+      <c r="S6" s="15"/>
+      <c r="T6" s="15"/>
+      <c r="U6" s="15">
         <f t="shared" ref="U6:U8" si="0">E6-SUM(G6:T6)</f>
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A7" s="22"/>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="s">
+    <row r="7" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A7" s="25"/>
+      <c r="B7" s="25"/>
+      <c r="C7" s="15" t="s">
         <v>42</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="15" t="s">
         <v>9</v>
       </c>
-      <c r="E7" s="23">
+      <c r="E7" s="15">
         <v>1</v>
       </c>
-      <c r="F7" s="23"/>
-      <c r="G7" s="23"/>
-      <c r="H7" s="23"/>
-      <c r="I7" s="23"/>
-      <c r="J7" s="23"/>
-      <c r="K7" s="23"/>
-      <c r="L7" s="23"/>
-      <c r="M7" s="23"/>
-      <c r="N7" s="23"/>
-      <c r="O7" s="23"/>
-      <c r="P7" s="23"/>
-      <c r="Q7" s="23"/>
-      <c r="R7" s="23"/>
-      <c r="S7" s="23"/>
-      <c r="T7" s="23"/>
-      <c r="U7" s="23">
+      <c r="F7" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="G7" s="15"/>
+      <c r="H7" s="15"/>
+      <c r="I7" s="15"/>
+      <c r="J7" s="15"/>
+      <c r="K7" s="15"/>
+      <c r="L7" s="15"/>
+      <c r="M7" s="15"/>
+      <c r="N7" s="15"/>
+      <c r="O7" s="15"/>
+      <c r="P7" s="15"/>
+      <c r="Q7" s="15"/>
+      <c r="R7" s="15"/>
+      <c r="S7" s="15"/>
+      <c r="T7" s="15"/>
+      <c r="U7" s="15">
         <f t="shared" si="0"/>
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A8" s="23" t="s">
+    <row r="8" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A8" s="15" t="s">
         <v>35</v>
       </c>
-      <c r="B8" s="23">
+      <c r="B8" s="15">
         <f>SUM(B5:B7)</f>
         <v>5</v>
       </c>
-      <c r="C8" s="24"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="23">
+      <c r="C8" s="16"/>
+      <c r="D8" s="16"/>
+      <c r="E8" s="15">
         <f>SUM(E5:E7)</f>
         <v>6</v>
       </c>
-      <c r="F8" s="24"/>
-      <c r="G8" s="23">
-        <f>SUM(G5:G7)</f>
+      <c r="F8" s="16"/>
+      <c r="G8" s="15">
+        <f t="shared" ref="G8:T8" si="1">SUM(G5:G7)</f>
         <v>0</v>
       </c>
-      <c r="H8" s="23">
-        <f>SUM(H5:H7)</f>
+      <c r="H8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="I8" s="23">
-        <f>SUM(I5:I7)</f>
+      <c r="I8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="J8" s="23">
-        <f>SUM(J5:J7)</f>
+      <c r="J8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="K8" s="23">
-        <f>SUM(K5:K7)</f>
+      <c r="K8" s="15">
+        <f t="shared" si="1"/>
+        <v>3</v>
+      </c>
+      <c r="L8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="L8" s="23">
-        <f>SUM(L5:L7)</f>
+      <c r="M8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="M8" s="23">
-        <f>SUM(M5:M7)</f>
+      <c r="N8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="N8" s="23">
-        <f>SUM(N5:N7)</f>
+      <c r="O8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="O8" s="23">
-        <f>SUM(O5:O7)</f>
+      <c r="P8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="P8" s="23">
-        <f>SUM(P5:P7)</f>
+      <c r="Q8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="Q8" s="23">
-        <f>SUM(Q5:Q7)</f>
+      <c r="R8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="R8" s="23">
-        <f>SUM(R5:R7)</f>
+      <c r="S8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="S8" s="23">
-        <f>SUM(S5:S7)</f>
+      <c r="T8" s="15">
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
-      <c r="T8" s="23">
-        <f>SUM(T5:T7)</f>
-        <v>0</v>
-      </c>
-      <c r="U8" s="23">
+      <c r="U8" s="15">
         <f t="shared" si="0"/>
-        <v>6</v>
+        <v>3</v>
       </c>
     </row>
-    <row r="9" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A9" s="25"/>
-      <c r="B9" s="25"/>
-      <c r="C9" s="25"/>
-      <c r="D9" s="25"/>
-      <c r="E9" s="23" t="s">
+    <row r="9" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A9" s="17"/>
+      <c r="B9" s="17"/>
+      <c r="C9" s="17"/>
+      <c r="D9" s="17"/>
+      <c r="E9" s="15" t="s">
         <v>36</v>
       </c>
-      <c r="F9" s="23">
+      <c r="F9" s="15">
         <f>SUM(E5:E7)</f>
         <v>6</v>
       </c>
-      <c r="G9" s="26">
+      <c r="G9" s="18">
         <f>F9-F9/14</f>
         <v>5.5714285714285712</v>
       </c>
-      <c r="H9" s="26">
+      <c r="H9" s="18">
         <f>G9-F9/14</f>
         <v>5.1428571428571423</v>
       </c>
-      <c r="I9" s="26">
+      <c r="I9" s="18">
         <f>H9-F9/14</f>
         <v>4.7142857142857135</v>
       </c>
-      <c r="J9" s="26">
+      <c r="J9" s="18">
         <f>I9-F9/14</f>
         <v>4.2857142857142847</v>
       </c>
-      <c r="K9" s="26">
+      <c r="K9" s="18">
         <f>J9-F9/14</f>
         <v>3.8571428571428563</v>
       </c>
-      <c r="L9" s="26">
+      <c r="L9" s="18">
         <f>K9-F9/14</f>
         <v>3.4285714285714279</v>
       </c>
-      <c r="M9" s="26">
+      <c r="M9" s="18">
         <f>L9-F9/14</f>
         <v>2.9999999999999996</v>
       </c>
-      <c r="N9" s="26">
+      <c r="N9" s="18">
         <f>M9-F9/14</f>
         <v>2.5714285714285712</v>
       </c>
-      <c r="O9" s="26">
+      <c r="O9" s="18">
         <f>N9-F9/14</f>
         <v>2.1428571428571428</v>
       </c>
-      <c r="P9" s="26">
+      <c r="P9" s="18">
         <f>O9-F9/14</f>
         <v>1.7142857142857142</v>
       </c>
-      <c r="Q9" s="26">
+      <c r="Q9" s="18">
         <f>P9-F9/14</f>
         <v>1.2857142857142856</v>
       </c>
-      <c r="R9" s="26">
+      <c r="R9" s="18">
         <f>Q9-F9/14</f>
         <v>0.85714285714285698</v>
       </c>
-      <c r="S9" s="26">
+      <c r="S9" s="18">
         <f>R9-F9/14</f>
         <v>0.42857142857142844</v>
       </c>
-      <c r="T9" s="26">
+      <c r="T9" s="18">
         <f>S9-F9/14</f>
         <v>0</v>
       </c>
-      <c r="U9" s="25"/>
+      <c r="U9" s="17"/>
     </row>
-    <row r="10" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A10" s="25"/>
-      <c r="B10" s="25"/>
-      <c r="C10" s="25"/>
-      <c r="D10" s="25"/>
-      <c r="E10" s="23" t="s">
+    <row r="10" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A10" s="17"/>
+      <c r="B10" s="17"/>
+      <c r="C10" s="17"/>
+      <c r="D10" s="17"/>
+      <c r="E10" s="15" t="s">
         <v>37</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="15">
         <f>SUM(E5:E7)</f>
         <v>6</v>
       </c>
-      <c r="G10" s="23">
-        <f>F10-SUM(G5:G7)</f>
+      <c r="G10" s="15">
+        <f t="shared" ref="G10:T10" si="2">F10-SUM(G5:G7)</f>
         <v>6</v>
       </c>
-      <c r="H10" s="23">
-        <f>G10-SUM(H5:H7)</f>
+      <c r="H10" s="15">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="I10" s="23">
-        <f>H10-SUM(I5:I7)</f>
+      <c r="I10" s="15">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="J10" s="23">
-        <f>I10-SUM(J5:J7)</f>
+      <c r="J10" s="15">
+        <f t="shared" si="2"/>
         <v>6</v>
       </c>
-      <c r="K10" s="23">
-        <f>J10-SUM(K5:K7)</f>
-        <v>6</v>
-      </c>
-      <c r="L10" s="23">
-        <f>K10-SUM(L5:L7)</f>
-        <v>6</v>
-      </c>
-      <c r="M10" s="23">
-        <f>L10-SUM(M5:M7)</f>
-        <v>6</v>
-      </c>
-      <c r="N10" s="23">
-        <f>M10-SUM(N5:N7)</f>
-        <v>6</v>
-      </c>
-      <c r="O10" s="23">
-        <f>N10-SUM(O5:O7)</f>
-        <v>6</v>
-      </c>
-      <c r="P10" s="23">
-        <f>O10-SUM(P5:P7)</f>
-        <v>6</v>
-      </c>
-      <c r="Q10" s="23">
-        <f>P10-SUM(Q5:Q7)</f>
-        <v>6</v>
-      </c>
-      <c r="R10" s="23">
-        <f>Q10-SUM(R5:R7)</f>
-        <v>6</v>
-      </c>
-      <c r="S10" s="23">
-        <f>R10-SUM(S5:S7)</f>
-        <v>6</v>
-      </c>
-      <c r="T10" s="23">
-        <f>S10-SUM(T5:T7)</f>
-        <v>6</v>
-      </c>
-      <c r="U10" s="25"/>
+      <c r="K10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="M10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="N10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="O10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="P10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="Q10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="R10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="S10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="T10" s="15">
+        <f t="shared" si="2"/>
+        <v>3</v>
+      </c>
+      <c r="U10" s="17"/>
     </row>
-    <row r="12" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A12" s="25"/>
-      <c r="B12" s="25"/>
-      <c r="C12" s="25"/>
-      <c r="D12" s="25"/>
+    <row r="12" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A12" s="17"/>
+      <c r="B12" s="17"/>
+      <c r="C12" s="17"/>
+      <c r="D12" s="17"/>
     </row>
-    <row r="13" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A13" s="25"/>
-      <c r="B13" s="25"/>
-      <c r="C13" s="25"/>
-      <c r="D13" s="25"/>
+    <row r="13" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A13" s="17"/>
+      <c r="B13" s="17"/>
+      <c r="C13" s="17"/>
+      <c r="D13" s="17"/>
     </row>
-    <row r="14" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A14" s="25"/>
-      <c r="B14" s="25"/>
-      <c r="C14" s="25"/>
-      <c r="D14" s="25"/>
+    <row r="14" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A14" s="17"/>
+      <c r="B14" s="17"/>
+      <c r="C14" s="17"/>
+      <c r="D14" s="17"/>
     </row>
-    <row r="15" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A15" s="25"/>
-      <c r="B15" s="25"/>
-      <c r="C15" s="25"/>
-      <c r="D15" s="25"/>
+    <row r="15" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A15" s="17"/>
+      <c r="B15" s="17"/>
+      <c r="C15" s="17"/>
+      <c r="D15" s="17"/>
     </row>
-    <row r="16" spans="1:21" x14ac:dyDescent="0.25">
-      <c r="A16" s="25"/>
-      <c r="B16" s="25"/>
-      <c r="C16" s="25"/>
-      <c r="D16" s="25"/>
+    <row r="16" spans="1:21" x14ac:dyDescent="0.3">
+      <c r="A16" s="17"/>
+      <c r="B16" s="17"/>
+      <c r="C16" s="17"/>
+      <c r="D16" s="17"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2573,18 +2607,18 @@
     <mergeCell ref="A5:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U8">
-    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>
@@ -2614,11 +2648,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView topLeftCell="A8" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>

</xml_diff>

<commit_message>
Updated sprint info, sprint8: added effort for fixing bug id25
</commit_message>
<xml_diff>
--- a/Documentation and designs/Sprint_info/Sprint8.xlsx
+++ b/Documentation and designs/Sprint_info/Sprint8.xlsx
@@ -421,22 +421,7 @@
     <cellStyle name="Accent6" xfId="2" builtinId="49"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="7">
-    <dxf>
-      <font>
-        <color rgb="FFC00000"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="9" tint="-0.499984740745262"/>
-      </font>
-    </dxf>
-    <dxf>
-      <font>
-        <color theme="7" tint="-0.24994659260841701"/>
-      </font>
-    </dxf>
+  <dxfs count="4">
     <dxf>
       <font>
         <color theme="0"/>
@@ -521,7 +506,6 @@
           </a:p>
         </c:rich>
       </c:tx>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -810,34 +794,34 @@
                   <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>3</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -858,11 +842,11 @@
           <c:showBubbleSize val="0"/>
         </c:dLbls>
         <c:smooth val="0"/>
-        <c:axId val="278370696"/>
-        <c:axId val="278371872"/>
+        <c:axId val="276447264"/>
+        <c:axId val="277341320"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="278370696"/>
+        <c:axId val="276447264"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -965,7 +949,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278371872"/>
+        <c:crossAx val="277341320"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -973,7 +957,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="278371872"/>
+        <c:axId val="277341320"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1018,7 +1002,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
           <c:spPr>
             <a:noFill/>
@@ -1077,7 +1060,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="278370696"/>
+        <c:crossAx val="276447264"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1740,7 +1723,7 @@
         <xdr:cNvPr id="3" name="Chart 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0200-000003000000}"/>
+              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0200-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2145,7 +2128,7 @@
   <dimension ref="A1:U16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F6" sqref="F6"/>
+      <selection activeCell="K7" sqref="K7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2306,7 +2289,9 @@
       <c r="H6" s="15"/>
       <c r="I6" s="15"/>
       <c r="J6" s="15"/>
-      <c r="K6" s="15"/>
+      <c r="K6" s="15">
+        <v>1</v>
+      </c>
       <c r="L6" s="15"/>
       <c r="M6" s="15"/>
       <c r="N6" s="15"/>
@@ -2318,7 +2303,7 @@
       <c r="T6" s="15"/>
       <c r="U6" s="15">
         <f t="shared" ref="U6:U8" si="0">E6-SUM(G6:T6)</f>
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="7" spans="1:21" x14ac:dyDescent="0.3">
@@ -2388,7 +2373,7 @@
       </c>
       <c r="K8" s="15">
         <f t="shared" si="1"/>
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="L8" s="15">
         <f t="shared" si="1"/>
@@ -2428,7 +2413,7 @@
       </c>
       <c r="U8" s="15">
         <f t="shared" si="0"/>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" spans="1:21" x14ac:dyDescent="0.3">
@@ -2531,43 +2516,43 @@
       </c>
       <c r="K10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="L10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="M10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="N10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="O10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="P10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="Q10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="R10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="S10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="T10" s="15">
         <f t="shared" si="2"/>
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="U10" s="17"/>
     </row>
@@ -2607,18 +2592,18 @@
     <mergeCell ref="A5:A7"/>
   </mergeCells>
   <conditionalFormatting sqref="F5:F7">
-    <cfRule type="cellIs" dxfId="6" priority="3" operator="equal">
+    <cfRule type="cellIs" dxfId="3" priority="3" operator="equal">
       <formula>"In progress"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="5" priority="5" operator="equal">
+    <cfRule type="cellIs" dxfId="2" priority="5" operator="equal">
       <formula>"Done"</formula>
     </cfRule>
-    <cfRule type="cellIs" dxfId="4" priority="6" operator="equal">
+    <cfRule type="cellIs" dxfId="1" priority="6" operator="equal">
       <formula>"To do"</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="U5:U8">
-    <cfRule type="cellIs" dxfId="3" priority="1" operator="greaterThan">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="greaterThan">
       <formula>0</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>